<commit_message>
edit main script and lookUp function, use string arrays for lookUp instead of pure tables
</commit_message>
<xml_diff>
--- a/test_partstracker.xlsx
+++ b/test_partstracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sue\Desktop\MakerSpace Fun\Random\Matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sue\Desktop\DBF 19-20 Docs\Matlab\parts-tracker-editor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0BB032-859C-46A0-8BE3-DCB4524AAAA9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B122D2-5328-47C7-945B-4F7E0E1A6EC6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{56E936FD-8488-44E9-816A-FEA4A1222563}"/>
   </bookViews>
@@ -471,9 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0AEE7CA-CA44-491C-88BF-BFB57C5933AF}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -481,6 +479,7 @@
     <col min="4" max="4" width="15.54296875" customWidth="1"/>
     <col min="5" max="5" width="17.6328125" customWidth="1"/>
     <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>